<commit_message>
primera clasifiacion estable solo faltan filtros de la tabla index
</commit_message>
<xml_diff>
--- a/sys/cla/files/claara/tplClasificacionMercanciasExport.xlsx
+++ b/sys/cla/files/claara/tplClasificacionMercanciasExport.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>REFERENCIA</t>
   </si>
@@ -48,9 +48,6 @@
     <t>FACTURA</t>
   </si>
   <si>
-    <t>AUTOR</t>
-  </si>
-  <si>
     <t>FRACCION</t>
   </si>
   <si>
@@ -58,6 +55,12 @@
   </si>
   <si>
     <t>CONSECUTIVO</t>
+  </si>
+  <si>
+    <t>EJECUTIVO</t>
+  </si>
+  <si>
+    <t>CLASIFICADOR</t>
   </si>
 </sst>
 </file>
@@ -119,8 +122,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -130,9 +135,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -411,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -429,10 +436,11 @@
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +451,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -455,20 +463,23 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1"/>
+  <autoFilter ref="A1:L1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>